<commit_message>
Interactive notebook active and usable
</commit_message>
<xml_diff>
--- a/app/documentation/example_expenses_en.xlsx
+++ b/app/documentation/example_expenses_en.xlsx
@@ -15,10 +15,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1613857134" val="980" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1613857134" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1613857134" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1613857134"/>
+      <pm:revision xmlns:pm="smNativeData" day="1614121310" val="980" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1614121310" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1614121310" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1614121310"/>
     </ext>
   </extLst>
 </workbook>
@@ -1285,7 +1285,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1613857134" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1614121310" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1300,7 +1300,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1613857134" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1614121310" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1316,7 +1316,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1613857134" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1614121310" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -1331,7 +1331,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1613857134" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1614121310" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="240" lang="default"/>
             <pm:ea face="Basic Roman" sz="240" lang="default"/>
@@ -1340,7 +1340,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1386,19 +1386,8 @@
     <fill>
       <patternFill patternType="none"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1613857134" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -1414,7 +1403,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613857134"/>
+          <pm:border xmlns:pm="smNativeData" id="1614121310"/>
         </ext>
       </extLst>
     </border>
@@ -1433,7 +1422,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613857134">
+          <pm:border xmlns:pm="smNativeData" id="1614121310">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1454,7 +1443,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613857134">
+          <pm:border xmlns:pm="smNativeData" id="1614121310">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1476,7 +1465,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613857134">
+          <pm:border xmlns:pm="smNativeData" id="1614121310">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1497,7 +1486,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613857134">
+          <pm:border xmlns:pm="smNativeData" id="1614121310">
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1518,7 +1507,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613857134">
+          <pm:border xmlns:pm="smNativeData" id="1614121310">
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1539,7 +1528,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613857134">
+          <pm:border xmlns:pm="smNativeData" id="1614121310">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1561,7 +1550,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613857134">
+          <pm:border xmlns:pm="smNativeData" id="1614121310">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1583,7 +1572,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613857134">
+          <pm:border xmlns:pm="smNativeData" id="1614121310">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -1606,7 +1595,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613857134">
+          <pm:border xmlns:pm="smNativeData" id="1614121310">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1628,7 +1617,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613857134">
+          <pm:border xmlns:pm="smNativeData" id="1614121310">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -1651,7 +1640,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613857134">
+          <pm:border xmlns:pm="smNativeData" id="1614121310">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1673,7 +1662,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613857134">
+          <pm:border xmlns:pm="smNativeData" id="1614121310">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1695,29 +1684,10 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613857134">
+          <pm:border xmlns:pm="smNativeData" id="1614121310">
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613857134"/>
         </ext>
       </extLst>
     </border>
@@ -1806,10 +1776,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1613857134" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1614121310" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1613857134" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1614121310" count="1">
         <pm:color name="Gris 20%" rgb="000000"/>
       </pm:colors>
     </ext>
@@ -2076,7 +2046,7 @@
   <dimension ref="A1:N624"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="B2" sqref="B2:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.553571" defaultRowHeight="15.40"/>
@@ -2088,20 +2058,8 @@
     <col min="6" max="6" width="14.330357" customWidth="1"/>
     <col min="7" max="7" width="10.544643" customWidth="1"/>
     <col min="8" max="8" width="25.214286" customWidth="1" style="27"/>
-    <col min="9" max="9" width="23.000000" hidden="1" customWidth="1">
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:columnDef xmlns:pm="smNativeData" id="1613857134" min="9" max="9" hidden="1" collapsedDB="0" collapsedOL="0"/>
-        </ext>
-      </extLst>
-    </col>
-    <col min="10" max="10" width="15.660714" hidden="1" customWidth="1">
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:columnDef xmlns:pm="smNativeData" id="1613857134" min="10" max="10" hidden="1" collapsedDB="0" collapsedOL="0"/>
-        </ext>
-      </extLst>
-    </col>
+    <col min="9" max="9" width="23.000000" customWidth="1"/>
+    <col min="10" max="10" width="15.660714" customWidth="1"/>
     <col min="12" max="12" width="18.437500" customWidth="1"/>
     <col min="13" max="13" width="13.107143" customWidth="1"/>
     <col min="14" max="14" width="14.000000" customWidth="1"/>
@@ -11919,7 +11877,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1613857134" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1614121310" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -11928,14 +11886,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1613857134" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1613857134" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1614121310" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1614121310" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1613857134" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614121310" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -11957,7 +11915,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1613857134" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1614121310" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -11966,14 +11924,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1613857134" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1613857134" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1614121310" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1614121310" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1613857134" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614121310" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -11995,7 +11953,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1613857134" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1614121310" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -12004,14 +11962,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1613857134" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1613857134" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1614121310" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1614121310" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1613857134" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614121310" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
The notebook now saves automatically into the raw_copied_excel file, but this slows a bit the reactions. This is something to regulate (save every 10 actions) ot to enhance in the future.
</commit_message>
<xml_diff>
--- a/app/documentation/example_expenses_en.xlsx
+++ b/app/documentation/example_expenses_en.xlsx
@@ -15,10 +15,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1614121310" val="980" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1614121310" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1614121310" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1614121310"/>
+      <pm:revision xmlns:pm="smNativeData" day="1614121623" val="980" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1614121623" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1614121623" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1614121623"/>
     </ext>
   </extLst>
 </workbook>
@@ -1285,7 +1285,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614121310" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1614121623" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1300,7 +1300,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614121310" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1614121623" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1316,7 +1316,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614121310" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1614121623" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -1331,7 +1331,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614121310" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1614121623" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="240" lang="default"/>
             <pm:ea face="Basic Roman" sz="240" lang="default"/>
@@ -1403,7 +1403,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614121310"/>
+          <pm:border xmlns:pm="smNativeData" id="1614121623"/>
         </ext>
       </extLst>
     </border>
@@ -1422,7 +1422,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614121310">
+          <pm:border xmlns:pm="smNativeData" id="1614121623">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1443,7 +1443,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614121310">
+          <pm:border xmlns:pm="smNativeData" id="1614121623">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1465,7 +1465,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614121310">
+          <pm:border xmlns:pm="smNativeData" id="1614121623">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1486,7 +1486,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614121310">
+          <pm:border xmlns:pm="smNativeData" id="1614121623">
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1507,7 +1507,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614121310">
+          <pm:border xmlns:pm="smNativeData" id="1614121623">
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1528,7 +1528,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614121310">
+          <pm:border xmlns:pm="smNativeData" id="1614121623">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1550,7 +1550,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614121310">
+          <pm:border xmlns:pm="smNativeData" id="1614121623">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1572,7 +1572,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614121310">
+          <pm:border xmlns:pm="smNativeData" id="1614121623">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -1595,7 +1595,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614121310">
+          <pm:border xmlns:pm="smNativeData" id="1614121623">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1617,7 +1617,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614121310">
+          <pm:border xmlns:pm="smNativeData" id="1614121623">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -1640,7 +1640,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614121310">
+          <pm:border xmlns:pm="smNativeData" id="1614121623">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1662,7 +1662,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614121310">
+          <pm:border xmlns:pm="smNativeData" id="1614121623">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1684,7 +1684,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614121310">
+          <pm:border xmlns:pm="smNativeData" id="1614121623">
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1776,10 +1776,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1614121310" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1614121623" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1614121310" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1614121623" count="1">
         <pm:color name="Gris 20%" rgb="000000"/>
       </pm:colors>
     </ext>
@@ -11877,7 +11877,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1614121310" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1614121623" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -11886,14 +11886,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1614121310" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1614121310" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1614121623" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1614121623" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614121310" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614121623" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -11915,7 +11915,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1614121310" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1614121623" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -11924,14 +11924,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1614121310" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1614121310" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1614121623" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1614121623" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614121310" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614121623" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -11953,7 +11953,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1614121310" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1614121623" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -11962,14 +11962,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1614121310" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1614121310" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1614121623" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1614121623" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614121310" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614121623" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
The backup of the buttons'text is now done using the internal dash persistence. If a problem raises because of it, it will always be possible to do the save manually using the already existing logic that was previously used.
</commit_message>
<xml_diff>
--- a/app/documentation/example_expenses_en.xlsx
+++ b/app/documentation/example_expenses_en.xlsx
@@ -15,10 +15,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1614466693" val="980" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1614466693" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1614466693" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1614466693"/>
+      <pm:revision xmlns:pm="smNativeData" day="1614502180" val="980" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1614502180" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1614502180" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1614502180"/>
     </ext>
   </extLst>
 </workbook>
@@ -1273,7 +1273,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614466693" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1614502180" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1288,7 +1288,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614466693" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1614502180" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1304,7 +1304,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614466693" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1614502180" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -1319,7 +1319,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614466693" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1614502180" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="240" lang="default"/>
             <pm:ea face="Basic Roman" sz="240" lang="default"/>
@@ -1376,7 +1376,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614466693"/>
+          <pm:border xmlns:pm="smNativeData" id="1614502180"/>
         </ext>
       </extLst>
     </border>
@@ -1395,7 +1395,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614466693">
+          <pm:border xmlns:pm="smNativeData" id="1614502180">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1416,7 +1416,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614466693">
+          <pm:border xmlns:pm="smNativeData" id="1614502180">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1438,7 +1438,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614466693">
+          <pm:border xmlns:pm="smNativeData" id="1614502180">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1459,7 +1459,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614466693">
+          <pm:border xmlns:pm="smNativeData" id="1614502180">
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1480,7 +1480,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614466693">
+          <pm:border xmlns:pm="smNativeData" id="1614502180">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1502,7 +1502,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614466693">
+          <pm:border xmlns:pm="smNativeData" id="1614502180">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -1525,7 +1525,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614466693">
+          <pm:border xmlns:pm="smNativeData" id="1614502180">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1547,7 +1547,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614466693">
+          <pm:border xmlns:pm="smNativeData" id="1614502180">
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1628,10 +1628,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1614466693" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1614502180" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1614466693" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1614502180" count="1">
         <pm:color name="Gris 20%" rgb="000000"/>
       </pm:colors>
     </ext>
@@ -9886,7 +9886,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1614466693" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1614502180" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -9895,14 +9895,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1614466693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1614466693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1614502180" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1614502180" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614466693" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614502180" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -9924,7 +9924,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1614466693" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1614502180" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -9933,14 +9933,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1614466693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1614466693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1614502180" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1614502180" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614466693" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614502180" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -9962,7 +9962,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1614466693" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1614502180" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -9971,14 +9971,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1614466693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1614466693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1614502180" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1614502180" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614466693" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614502180" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>